<commit_message>
holdover testing data from October
</commit_message>
<xml_diff>
--- a/Mandarin_Stims.xlsx
+++ b/Mandarin_Stims.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/callab2/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6C17D225-8DC4-594B-B39D-DC651E1E1184}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="2580" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BF2EFBA6-13B4-5045-AD25-040A416C02E3}"/>
+    <workbookView xWindow="6460" yWindow="2580" windowWidth="28040" windowHeight="17440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="Mandarin" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Row #</t>
   </si>
@@ -101,18 +98,31 @@
   </si>
   <si>
     <t>老虎在喝水吗？</t>
+  </si>
+  <si>
+    <t>trial1</t>
+  </si>
+  <si>
+    <t>trial2</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>trialNum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -198,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -250,7 +260,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -444,26 +454,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBC9460-1C14-EF46-8829-D996391304EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="4" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,61 +501,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -553,38 +563,43 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25481615-4C6F-A44B-AE55-DCFF7397428C}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -598,7 +613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -613,9 +628,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -628,7 +643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -643,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -658,7 +673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -673,37 +688,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>